<commit_message>
edited html file for ranking list template
</commit_message>
<xml_diff>
--- a/staticfiles/excel/Overall Rank.xlsx
+++ b/staticfiles/excel/Overall Rank.xlsx
@@ -13,10 +13,10 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1698617482" val="1066" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1698617482" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1698617482" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1698617482"/>
+      <pm:revision xmlns:pm="smNativeData" day="1700807062" val="1066" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1700807062" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1700807062" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1700807062"/>
     </ext>
   </extLst>
 </workbook>
@@ -52,28 +52,52 @@
     <t>ʸᵍᵒ ᴇʀɪs°</t>
   </si>
   <si>
+    <t>Kryztyn Cordero</t>
+  </si>
+  <si>
+    <t>ƚყɳ</t>
+  </si>
+  <si>
+    <t>Ian Gerome Alumno</t>
+  </si>
+  <si>
+    <t>IanTzy God Mode</t>
+  </si>
+  <si>
+    <t>Patrick Fermanes</t>
+  </si>
+  <si>
+    <t>Paᴛʀick God Mode</t>
+  </si>
+  <si>
+    <t>Gray Plays</t>
+  </si>
+  <si>
+    <t>ɢʀᴀʏ</t>
+  </si>
+  <si>
+    <t>Anjelou F. Naong</t>
+  </si>
+  <si>
+    <t>Aeon</t>
+  </si>
+  <si>
     <t>Prince Nitsuga</t>
   </si>
   <si>
     <t>Aj Prince</t>
   </si>
   <si>
-    <t>Ian Gerome Alumno</t>
-  </si>
-  <si>
-    <t>IanTzy God Mode</t>
-  </si>
-  <si>
     <t>Emz M. Cinco</t>
   </si>
   <si>
     <t>repadz04</t>
   </si>
   <si>
-    <t>Patrick Fermanes</t>
-  </si>
-  <si>
-    <t>Paᴛʀick God Mode</t>
+    <t>Renz Silang Rico</t>
+  </si>
+  <si>
+    <t>Maldito</t>
   </si>
   <si>
     <t>Choii Zhee</t>
@@ -82,16 +106,49 @@
     <t>Kurdapyo</t>
   </si>
   <si>
-    <t>Gray Plays</t>
-  </si>
-  <si>
-    <t>ɢʀᴀʏ</t>
-  </si>
-  <si>
-    <t>Anjelou F. Naong</t>
-  </si>
-  <si>
-    <t>Aeon</t>
+    <t>Jd Pedraja</t>
+  </si>
+  <si>
+    <t>Shantidolph</t>
+  </si>
+  <si>
+    <t>Jaylord Sanchez Cabije</t>
+  </si>
+  <si>
+    <t>ST★RKING</t>
+  </si>
+  <si>
+    <t>Noelito De Gracia</t>
+  </si>
+  <si>
+    <t>Enelsuu.</t>
+  </si>
+  <si>
+    <t>Yoon Ei</t>
+  </si>
+  <si>
+    <t>Xyvian Shane Gera Tia</t>
+  </si>
+  <si>
+    <t>Sʜᴇɴɢ♡</t>
+  </si>
+  <si>
+    <t>U Aung Kyaw Soe</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>Clyde Morcillos</t>
+  </si>
+  <si>
+    <t>ᴮᶠᵁUNLOVED</t>
+  </si>
+  <si>
+    <t>Jundel Palma</t>
+  </si>
+  <si>
+    <t>Sukol DAW Beh</t>
   </si>
   <si>
     <t>Piolo A Aguilera</t>
@@ -100,31 +157,28 @@
     <t>Sʜaɴᴇ♡</t>
   </si>
   <si>
-    <t>Renz Silang Rico</t>
-  </si>
-  <si>
-    <t>Maldito</t>
-  </si>
-  <si>
-    <t>Yoon Ei</t>
-  </si>
-  <si>
-    <t>Clyde Morcillos</t>
-  </si>
-  <si>
-    <t>ᴮᶠᵁUNLOVED</t>
-  </si>
-  <si>
-    <t>Xyvian Shane Gera Tia</t>
-  </si>
-  <si>
-    <t>Sʜᴇɴɢ♡</t>
-  </si>
-  <si>
-    <t>Noelito De Gracia</t>
-  </si>
-  <si>
-    <t>Enelsuu.</t>
+    <t>Edgardo Estrada</t>
+  </si>
+  <si>
+    <t>EdStronG</t>
+  </si>
+  <si>
+    <t>Melvin Abilong</t>
+  </si>
+  <si>
+    <t>EGGPLANT GAMING</t>
+  </si>
+  <si>
+    <t>Sharwin Paolo Cabataña</t>
+  </si>
+  <si>
+    <t>Lewenzeith D. Pelaez</t>
+  </si>
+  <si>
+    <t>Teejay Caraan</t>
+  </si>
+  <si>
+    <t>makisig</t>
   </si>
   <si>
     <t>Skidamarink Arellano</t>
@@ -133,22 +187,34 @@
     <t>MikeeMike</t>
   </si>
   <si>
-    <t>U Aung Kyaw Soe</t>
-  </si>
-  <si>
-    <t>Leon</t>
-  </si>
-  <si>
-    <t>Jd Pedraja</t>
-  </si>
-  <si>
-    <t>Shantidolph</t>
-  </si>
-  <si>
-    <t>Jundel Palma</t>
-  </si>
-  <si>
-    <t>Sukol DAW Beh</t>
+    <t>Oliveranz Alvarez</t>
+  </si>
+  <si>
+    <t>fluffybok</t>
+  </si>
+  <si>
+    <t>Joshua Villegas</t>
+  </si>
+  <si>
+    <t>ʏᴏɴᴋᴏ Shanks</t>
+  </si>
+  <si>
+    <t>Relly H. Medina</t>
+  </si>
+  <si>
+    <t>ᴵᴱ°HowMuch</t>
+  </si>
+  <si>
+    <t>Enry Charles Bernardo</t>
+  </si>
+  <si>
+    <t>Ryy.</t>
+  </si>
+  <si>
+    <t>Jomailyn Fay P. Aguilar</t>
+  </si>
+  <si>
+    <t>Star18</t>
   </si>
   <si>
     <t>Christian Nevado</t>
@@ -157,18 +223,6 @@
     <t>av⁰² Jinx</t>
   </si>
   <si>
-    <t>Oliveranz Alvarez</t>
-  </si>
-  <si>
-    <t>fluffybok</t>
-  </si>
-  <si>
-    <t>Kryztyn Cordero</t>
-  </si>
-  <si>
-    <t>ƚყɳ</t>
-  </si>
-  <si>
     <t>Limar N.Ramis</t>
   </si>
   <si>
@@ -181,12 +235,6 @@
     <t>MAGNUS</t>
   </si>
   <si>
-    <t>Jaylord Sanchez Cabije</t>
-  </si>
-  <si>
-    <t>ST★RKING</t>
-  </si>
-  <si>
     <t>Jay-ar Villarin Sacayan</t>
   </si>
   <si>
@@ -205,40 +253,16 @@
     <t>AS.Briii</t>
   </si>
   <si>
-    <t>Joshua Villegas</t>
-  </si>
-  <si>
-    <t>ʏᴏɴᴋᴏ Shanks</t>
-  </si>
-  <si>
-    <t>Melvin Abilong</t>
-  </si>
-  <si>
-    <t>EGGPLANT GAMING</t>
-  </si>
-  <si>
-    <t>Sharwin Paolo Cabataña</t>
-  </si>
-  <si>
-    <t>Lewenzeith D. Pelaez</t>
-  </si>
-  <si>
-    <t>Enry Charles Bernardo</t>
-  </si>
-  <si>
-    <t>Ryy.</t>
-  </si>
-  <si>
-    <t>Jomailyn Fay P. Aguilar</t>
-  </si>
-  <si>
-    <t>Star18</t>
-  </si>
-  <si>
-    <t>Edgardo Estrada</t>
-  </si>
-  <si>
-    <t>EdStronG</t>
+    <t>Kevin Ongjunco</t>
+  </si>
+  <si>
+    <t>{†KILLAZ†}</t>
+  </si>
+  <si>
+    <t>Xanuel Mark Beatingo</t>
+  </si>
+  <si>
+    <t>ᴘᴏᴘᴏ</t>
   </si>
   <si>
     <t>John Dave V. Lazaga</t>
@@ -247,28 +271,22 @@
     <t>jd gwapo</t>
   </si>
   <si>
+    <t>Socorro Reyes</t>
+  </si>
+  <si>
+    <t>Soki71</t>
+  </si>
+  <si>
     <t>Real Spencer</t>
   </si>
   <si>
     <t>ʸᵍᵒ ᴇᴀʀʟ</t>
   </si>
   <si>
-    <t>Kevin Ongjunco</t>
-  </si>
-  <si>
-    <t>{†KILLAZ†}</t>
-  </si>
-  <si>
-    <t>Teejay Caraan</t>
-  </si>
-  <si>
-    <t>makisig</t>
-  </si>
-  <si>
-    <t>Relly H. Medina</t>
-  </si>
-  <si>
-    <t>ᴵᴱ°HowMuch</t>
+    <t>Jayson Pogoy</t>
+  </si>
+  <si>
+    <t>Flux.</t>
   </si>
   <si>
     <t>Yoko Na</t>
@@ -277,36 +295,36 @@
     <t>Naga Siren</t>
   </si>
   <si>
+    <t>Rey Q Ibañez</t>
+  </si>
+  <si>
+    <t>ZenabiRhey</t>
+  </si>
+  <si>
+    <t>RM Capulong</t>
+  </si>
+  <si>
+    <t>mariepeng</t>
+  </si>
+  <si>
     <t>Jay Paul Butad</t>
   </si>
   <si>
     <t>I'll roam</t>
   </si>
   <si>
-    <t>Xanuel Mark Beatingo</t>
-  </si>
-  <si>
-    <t>ᴘᴏᴘᴏ</t>
-  </si>
-  <si>
-    <t>Socorro Reyes</t>
-  </si>
-  <si>
-    <t>Soki71</t>
-  </si>
-  <si>
-    <t>Rey Q Ibañez</t>
-  </si>
-  <si>
-    <t>ZenabiRhey</t>
-  </si>
-  <si>
     <t>Jay C. Montes</t>
   </si>
   <si>
     <t>SIKAD</t>
   </si>
   <si>
+    <t>Bobot Solano</t>
+  </si>
+  <si>
+    <t>Yoshi</t>
+  </si>
+  <si>
     <t>Paolo Biscayda</t>
   </si>
   <si>
@@ -325,12 +343,6 @@
     <t>Ishie.</t>
   </si>
   <si>
-    <t>RM Capulong</t>
-  </si>
-  <si>
-    <t>mariepeng</t>
-  </si>
-  <si>
     <t>Rowie Gell Gallego</t>
   </si>
   <si>
@@ -383,18 +395,6 @@
   </si>
   <si>
     <t>Jinny</t>
-  </si>
-  <si>
-    <t>Jayson Pogoy</t>
-  </si>
-  <si>
-    <t>Flux.</t>
-  </si>
-  <si>
-    <t>Bobot Solano</t>
-  </si>
-  <si>
-    <t>Yoshi</t>
   </si>
   <si>
     <t>Ely John Guevarra</t>
@@ -450,7 +450,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1698617482" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700807062" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -483,7 +483,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1698617482"/>
+          <pm:border xmlns:pm="smNativeData" id="1700807062"/>
         </ext>
       </extLst>
     </border>
@@ -501,7 +501,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1698617482" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1700807062" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -768,7 +768,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -810,13 +810,13 @@
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>416</v>
+        <v>498</v>
       </c>
       <c r="E2" t="n">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F2" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -833,16 +833,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>397</v>
+        <v>468</v>
       </c>
       <c r="E3" t="n">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="F3" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -856,16 +856,16 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>372</v>
+        <v>459</v>
       </c>
       <c r="E4" t="n">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F4" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -879,16 +879,16 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>302</v>
+        <v>499</v>
       </c>
       <c r="E5" t="n">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F5" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G5" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -902,16 +902,16 @@
         <v>16</v>
       </c>
       <c r="D6" t="n">
-        <v>444</v>
+        <v>381</v>
       </c>
       <c r="E6" t="n">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F6" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -925,16 +925,16 @@
         <v>18</v>
       </c>
       <c r="D7" t="n">
-        <v>314</v>
+        <v>360</v>
       </c>
       <c r="E7" t="n">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F7" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -948,16 +948,16 @@
         <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>307</v>
+        <v>439</v>
       </c>
       <c r="E8" t="n">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F8" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G8" t="n">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -971,16 +971,16 @@
         <v>22</v>
       </c>
       <c r="D9" t="n">
-        <v>289</v>
+        <v>347</v>
       </c>
       <c r="E9" t="n">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F9" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9" t="n">
-        <v>7</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -994,16 +994,16 @@
         <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>373</v>
+        <v>477</v>
       </c>
       <c r="E10" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F10" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G10" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1017,16 +1017,16 @@
         <v>26</v>
       </c>
       <c r="D11" t="n">
-        <v>395</v>
+        <v>351</v>
       </c>
       <c r="E11" t="n">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F11" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G11" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1037,16 +1037,16 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" t="n">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="E12" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F12" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12" t="n">
         <v>6</v>
@@ -1057,22 +1057,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>347</v>
+        <v>316</v>
       </c>
       <c r="E13" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F13" t="n">
         <v>34</v>
       </c>
       <c r="G13" t="n">
-        <v>-8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1080,19 +1080,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="n">
-        <v>286</v>
+        <v>356</v>
       </c>
       <c r="E14" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F14" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1103,22 +1103,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="D15" t="n">
-        <v>303</v>
+        <v>466</v>
       </c>
       <c r="E15" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F15" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G15" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1132,16 +1132,16 @@
         <v>35</v>
       </c>
       <c r="D16" t="n">
-        <v>281</v>
+        <v>323</v>
       </c>
       <c r="E16" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F16" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G16" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1155,16 +1155,16 @@
         <v>37</v>
       </c>
       <c r="D17" t="n">
-        <v>261</v>
+        <v>318</v>
       </c>
       <c r="E17" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F17" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G17" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1178,16 +1178,16 @@
         <v>39</v>
       </c>
       <c r="D18" t="n">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="E18" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F18" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G18" t="n">
-        <v>10</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1201,16 +1201,16 @@
         <v>41</v>
       </c>
       <c r="D19" t="n">
-        <v>312</v>
+        <v>364</v>
       </c>
       <c r="E19" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F19" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G19" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1224,16 +1224,16 @@
         <v>43</v>
       </c>
       <c r="D20" t="n">
-        <v>301</v>
+        <v>373</v>
       </c>
       <c r="E20" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F20" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G20" t="n">
-        <v>-1</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1247,16 +1247,16 @@
         <v>45</v>
       </c>
       <c r="D21" t="n">
-        <v>282</v>
+        <v>330</v>
       </c>
       <c r="E21" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F21" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G21" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1270,16 +1270,16 @@
         <v>47</v>
       </c>
       <c r="D22" t="n">
-        <v>270</v>
+        <v>331</v>
       </c>
       <c r="E22" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F22" t="n">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G22" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="D23" t="n">
-        <v>264</v>
+        <v>330</v>
       </c>
       <c r="E23" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F23" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="G23" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1319,13 +1319,13 @@
         <v>319</v>
       </c>
       <c r="E24" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F24" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G24" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1339,16 +1339,16 @@
         <v>53</v>
       </c>
       <c r="D25" t="n">
-        <v>226</v>
+        <v>318</v>
       </c>
       <c r="E25" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F25" t="n">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G25" t="n">
-        <v>-4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1362,16 +1362,16 @@
         <v>55</v>
       </c>
       <c r="D26" t="n">
-        <v>281</v>
+        <v>316</v>
       </c>
       <c r="E26" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F26" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G26" t="n">
-        <v>-15</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1385,16 +1385,16 @@
         <v>57</v>
       </c>
       <c r="D27" t="n">
-        <v>274</v>
+        <v>403</v>
       </c>
       <c r="E27" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F27" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G27" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1408,16 +1408,16 @@
         <v>59</v>
       </c>
       <c r="D28" t="n">
-        <v>256</v>
+        <v>299</v>
       </c>
       <c r="E28" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F28" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1431,16 +1431,16 @@
         <v>61</v>
       </c>
       <c r="D29" t="n">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="E29" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F29" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G29" t="n">
-        <v>-5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1454,16 +1454,16 @@
         <v>63</v>
       </c>
       <c r="D30" t="n">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="E30" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F30" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G30" t="n">
-        <v>-5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1477,16 +1477,16 @@
         <v>65</v>
       </c>
       <c r="D31" t="n">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="E31" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F31" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G31" t="n">
-        <v>-4</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1500,16 +1500,16 @@
         <v>67</v>
       </c>
       <c r="D32" t="n">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="E32" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F32" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G32" t="n">
-        <v>-2</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1523,16 +1523,16 @@
         <v>69</v>
       </c>
       <c r="D33" t="n">
-        <v>266</v>
+        <v>319</v>
       </c>
       <c r="E33" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F33" t="n">
         <v>30</v>
       </c>
       <c r="G33" t="n">
-        <v>-4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1546,16 +1546,16 @@
         <v>71</v>
       </c>
       <c r="D34" t="n">
-        <v>225</v>
+        <v>281</v>
       </c>
       <c r="E34" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F34" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G34" t="n">
-        <v>-2</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1569,16 +1569,16 @@
         <v>73</v>
       </c>
       <c r="D35" t="n">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="E35" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F35" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G35" t="n">
-        <v>16</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1592,16 +1592,16 @@
         <v>75</v>
       </c>
       <c r="D36" t="n">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="E36" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F36" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G36" t="n">
-        <v>-2</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1615,16 +1615,16 @@
         <v>77</v>
       </c>
       <c r="D37" t="n">
-        <v>268</v>
+        <v>305</v>
       </c>
       <c r="E37" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F37" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G37" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1638,16 +1638,16 @@
         <v>79</v>
       </c>
       <c r="D38" t="n">
-        <v>220</v>
+        <v>319</v>
       </c>
       <c r="E38" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F38" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G38" t="n">
-        <v>-2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1661,16 +1661,16 @@
         <v>81</v>
       </c>
       <c r="D39" t="n">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E39" t="n">
+        <v>36</v>
+      </c>
+      <c r="F39" t="n">
         <v>31</v>
       </c>
-      <c r="F39" t="n">
-        <v>23</v>
-      </c>
       <c r="G39" t="n">
-        <v>-13</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1684,16 +1684,16 @@
         <v>83</v>
       </c>
       <c r="D40" t="n">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="E40" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F40" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G40" t="n">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1707,16 +1707,16 @@
         <v>85</v>
       </c>
       <c r="D41" t="n">
-        <v>184</v>
+        <v>270</v>
       </c>
       <c r="E41" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F41" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G41" t="n">
-        <v>-2</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1730,16 +1730,16 @@
         <v>87</v>
       </c>
       <c r="D42" t="n">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E42" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F42" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G42" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1753,16 +1753,16 @@
         <v>89</v>
       </c>
       <c r="D43" t="n">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E43" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F43" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G43" t="n">
-        <v>6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1776,16 +1776,16 @@
         <v>91</v>
       </c>
       <c r="D44" t="n">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="E44" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F44" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1799,16 +1799,16 @@
         <v>93</v>
       </c>
       <c r="D45" t="n">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="E45" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F45" t="n">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G45" t="n">
-        <v>-5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1822,13 +1822,13 @@
         <v>95</v>
       </c>
       <c r="D46" t="n">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="E46" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F46" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G46" t="n">
         <v>-5</v>
@@ -1845,16 +1845,16 @@
         <v>97</v>
       </c>
       <c r="D47" t="n">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="E47" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F47" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G47" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1868,16 +1868,16 @@
         <v>99</v>
       </c>
       <c r="D48" t="n">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E48" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F48" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G48" t="n">
-        <v>-4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1891,16 +1891,16 @@
         <v>101</v>
       </c>
       <c r="D49" t="n">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E49" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F49" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G49" t="n">
-        <v>9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1914,16 +1914,16 @@
         <v>103</v>
       </c>
       <c r="D50" t="n">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E50" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F50" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G50" t="n">
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1937,16 +1937,16 @@
         <v>105</v>
       </c>
       <c r="D51" t="n">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E51" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F51" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G51" t="n">
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1960,16 +1960,16 @@
         <v>107</v>
       </c>
       <c r="D52" t="n">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E52" t="n">
         <v>22</v>
       </c>
       <c r="F52" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G52" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1983,16 +1983,16 @@
         <v>109</v>
       </c>
       <c r="D53" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E53" t="n">
         <v>22</v>
       </c>
       <c r="F53" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G53" t="n">
-        <v>7</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2006,16 +2006,16 @@
         <v>111</v>
       </c>
       <c r="D54" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E54" t="n">
         <v>22</v>
       </c>
       <c r="F54" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G54" t="n">
-        <v>5</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2029,16 +2029,16 @@
         <v>113</v>
       </c>
       <c r="D55" t="n">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="E55" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F55" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G55" t="n">
-        <v>-5</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2052,16 +2052,16 @@
         <v>115</v>
       </c>
       <c r="D56" t="n">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="E56" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F56" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G56" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2075,16 +2075,16 @@
         <v>117</v>
       </c>
       <c r="D57" t="n">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E57" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F57" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G57" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2098,16 +2098,16 @@
         <v>119</v>
       </c>
       <c r="D58" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E58" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F58" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G58" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2121,16 +2121,16 @@
         <v>121</v>
       </c>
       <c r="D59" t="n">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E59" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F59" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G59" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2144,16 +2144,16 @@
         <v>123</v>
       </c>
       <c r="D60" t="n">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="E60" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F60" t="n">
         <v>16</v>
       </c>
       <c r="G60" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2176,7 +2176,7 @@
         <v>32</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2199,7 +2199,7 @@
         <v>5</v>
       </c>
       <c r="G62" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2275,7 +2275,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1698617482" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1700807062" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2284,16 +2284,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1698617482" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1698617482" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1698617482" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1698617482" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1700807062" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1700807062" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1700807062" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1700807062" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1698617482" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1700807062" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>